<commit_message>
added report for submission
</commit_message>
<xml_diff>
--- a/Projects/2_Classical Planning/experiments/workstation.xlsx
+++ b/Projects/2_Classical Planning/experiments/workstation.xlsx
@@ -5,18 +5,67 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Extended/Users/yhbyhb/Documents/GitHub/artificial-intelligence/Projects/2_Classical Planning/experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhbyhb/Documents/GitHub/artificial-intelligence/Projects/2_Classical Planning/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FB9D33A-BD54-4248-B325-7ECAC07A680A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7D6CF8E5-AD49-0947-A019-020E4AA2D7CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="5520" windowWidth="29840" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workstation" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">workstation!$A$1:$J$45</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">workstation!$E$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">workstation!$E$2:$E$45</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">workstation!$J$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">workstation!$J$2:$J$45</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">workstation!$E$2:$E$45</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">workstation!$F$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">workstation!$F$2:$F$45</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">workstation!$G$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">workstation!$G$2:$G$45</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">workstation!$H$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">workstation!$H$2:$H$45</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">workstation!$I$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">workstation!$F$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">workstation!$I$2:$I$45</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">workstation!$J$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">workstation!$J$2:$J$45</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">workstation!$E$2:$E$45</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">workstation!$F$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">workstation!$F$2:$F$45</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">workstation!$G$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">workstation!$G$2:$G$45</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">workstation!$H$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">workstation!$H$2:$H$45</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">workstation!$F$2:$F$45</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">workstation!$I$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">workstation!$I$2:$I$45</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">workstation!$J$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">workstation!$J$2:$J$45</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">workstation!$D$26</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">workstation!$D$4</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">workstation!$E$26:$E$42</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">workstation!$E$2:$E$45</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">workstation!$E$4:$E$20</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">workstation!$F$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">workstation!$G$1</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">workstation!$F$2:$F$45</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">workstation!$G$1</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">workstation!$G$2:$G$45</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">workstation!$H$1</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">workstation!$H$2:$H$45</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">workstation!$I$1</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">workstation!$I$2:$I$45</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">workstation!$J$26:$J$42</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">workstation!$J$4:$J$20</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">workstation!$G$2:$G$45</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">workstation!$H$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">workstation!$H$2:$H$45</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">workstation!$I$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">workstation!$I$2:$I$45</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -109,6 +158,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -586,8 +638,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -644,6 +697,2550 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time elapsed by</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0%"/>
+              <a:t> Actions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>workstation!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uniform_cost_search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>workstation!$E$4:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>workstation!$J$4:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4952100000063999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54749859999992601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2738130000000101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7705774000000902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C2F6-F445-B2BF-7C0ED512F3C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>workstation!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>astar_search with h_unmet_goals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>workstation!$E$31:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>workstation!$J$31:$J$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.57154000000809E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.612316599999985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95949679999989701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8185496999999402</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C2F6-F445-B2BF-7C0ED512F3C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>workstation!$D$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy_best_first_graph_search with h_unmet_goals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>workstation!$E$16:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>workstation!$J$16:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0289999999458797E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1319000000166797E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5544500000014502E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2110000000320703E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C2F6-F445-B2BF-7C0ED512F3C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="793122927"/>
+        <c:axId val="792817103"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="793122927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65%"/>
+                        <a:lumOff val="35%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Actions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65%"/>
+                      <a:lumOff val="35%"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="792817103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="792817103"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65%"/>
+                        <a:lumOff val="35%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time elapsed (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65%"/>
+                      <a:lumOff val="35%"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="793122927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15%"/>
+          <a:lumOff val="85%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Expansions</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0%"/>
+              <a:t> by Actions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>workstation!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>uniform_cost_search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>workstation!$E$4:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>workstation!$F$4:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18510</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7868-D74B-8476-5617753B486C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>workstation!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>astar_search with h_unmet_goals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>workstation!$E$31:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>workstation!$F$31:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2467</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7388</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7868-D74B-8476-5617753B486C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>workstation!$D$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greedy_best_first_graph_search with h_unmet_goals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>workstation!$E$16:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>workstation!$F$16:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7868-D74B-8476-5617753B486C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="793122927"/>
+        <c:axId val="792817103"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="793122927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65%"/>
+                        <a:lumOff val="35%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR"/>
+                  <a:t>Actions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65%"/>
+                      <a:lumOff val="35%"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="792817103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="792817103"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65%"/>
+                        <a:lumOff val="35%"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Expansions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65%"/>
+                      <a:lumOff val="35%"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25%"/>
+                <a:lumOff val="75%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="793122927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15%"/>
+          <a:lumOff val="85%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+    <a:lumOff val="20%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+    <a:lumOff val="40%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+    <a:lumOff val="30%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+    <a:lumOff val="50%"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+    <a:lumOff val="20%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+    <a:lumOff val="40%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+    <a:lumOff val="30%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+    <a:lumOff val="50%"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75%"/>
+        <a:lumOff val="25%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75%"/>
+          <a:lumOff val="25%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5%"/>
+            <a:lumOff val="95%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50%"/>
+            <a:lumOff val="50%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75%"/>
+        <a:lumOff val="25%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75%"/>
+          <a:lumOff val="25%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5%"/>
+            <a:lumOff val="95%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50%"/>
+            <a:lumOff val="50%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BD2C6E1-6F0D-D24B-86C4-7AB1C9234423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9759E71A-D625-AC41-B0C3-606F6F6003A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -943,10 +3540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,7 +3553,9 @@
     <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -986,11 +3586,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1018,11 +3618,11 @@
       <c r="I2">
         <v>6</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>1.9652400000040801E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1050,7 +3650,7 @@
       <c r="I3">
         <v>20</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>8.9427999998861196E-3</v>
       </c>
     </row>
@@ -1082,43 +3682,43 @@
       <c r="I4">
         <v>6</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>2.4952100000063999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>5154</v>
       </c>
       <c r="G5">
+        <v>5156</v>
+      </c>
+      <c r="H5">
+        <v>46618</v>
+      </c>
+      <c r="I5">
         <v>9</v>
       </c>
-      <c r="H5">
-        <v>29</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>4.0289999999458797E-3</v>
+      <c r="J5" s="1">
+        <v>0.54749859999992601</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1146,11 +3746,11 @@
       <c r="I6">
         <v>6</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>0.23699759999999501</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1178,11 +3778,11 @@
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>0.13018080000006099</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1210,43 +3810,43 @@
       <c r="I8">
         <v>6</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>0.57049379999989402</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="F9">
-        <v>50</v>
+        <v>18510</v>
       </c>
       <c r="G9">
-        <v>52</v>
+        <v>18512</v>
       </c>
       <c r="H9">
-        <v>206</v>
+        <v>161936</v>
       </c>
       <c r="I9">
-        <v>6</v>
-      </c>
-      <c r="J9">
-        <v>2.57154000000809E-2</v>
+        <v>12</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.2738130000000101</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1274,11 +3874,11 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>0.50718449999999304</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1306,11 +3906,11 @@
       <c r="I11">
         <v>6</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>0.34311809999985599</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1338,11 +3938,11 @@
       <c r="I12">
         <v>6</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>0.92176220000010201</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1370,11 +3970,11 @@
       <c r="I13">
         <v>9</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>0.29218879999984798</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1402,75 +4002,75 @@
       <c r="I14">
         <v>619</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>0.52901729999985003</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="F15">
-        <v>5154</v>
+        <v>113339</v>
       </c>
       <c r="G15">
-        <v>5156</v>
+        <v>113341</v>
       </c>
       <c r="H15">
-        <v>46618</v>
+        <v>1066413</v>
       </c>
       <c r="I15">
-        <v>9</v>
-      </c>
-      <c r="J15">
-        <v>0.54749859999992601</v>
+        <v>14</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7.7705774000000902</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G16">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H16">
-        <v>170</v>
+        <v>29</v>
       </c>
       <c r="I16">
-        <v>9</v>
-      </c>
-      <c r="J16">
-        <v>3.1319000000166797E-2</v>
+        <v>6</v>
+      </c>
+      <c r="J16" s="1">
+        <v>4.0289999999458797E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1498,11 +4098,11 @@
       <c r="I17">
         <v>9</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>0.87920749999989301</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1530,11 +4130,11 @@
       <c r="I18">
         <v>9</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <v>0.72667299999989099</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1562,7 +4162,7 @@
       <c r="I19">
         <v>9</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="1">
         <v>2.2095773999999402</v>
       </c>
     </row>
@@ -1571,34 +4171,34 @@
         <v>2</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E20">
         <v>72</v>
       </c>
       <c r="F20">
-        <v>2467</v>
+        <v>17</v>
       </c>
       <c r="G20">
-        <v>2469</v>
+        <v>19</v>
       </c>
       <c r="H20">
-        <v>22522</v>
+        <v>170</v>
       </c>
       <c r="I20">
         <v>9</v>
       </c>
-      <c r="J20">
-        <v>0.612316599999985</v>
+      <c r="J20" s="1">
+        <v>3.1319000000166797E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1626,11 +4226,11 @@
       <c r="I21">
         <v>9</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="1">
         <v>11.1266611999999</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1658,11 +4258,11 @@
       <c r="I22">
         <v>9</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
         <v>26.4144266999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1690,11 +4290,11 @@
       <c r="I23">
         <v>9</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
         <v>98.161397500000007</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1722,11 +4322,11 @@
       <c r="I24">
         <v>12</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="1">
         <v>0.85814200000004304</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1754,7 +4354,7 @@
       <c r="I25">
         <v>392</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="1">
         <v>0.23960110000007201</v>
       </c>
     </row>
@@ -1763,66 +4363,66 @@
         <v>3</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E26">
         <v>88</v>
       </c>
       <c r="F26">
-        <v>18510</v>
+        <v>25</v>
       </c>
       <c r="G26">
-        <v>18512</v>
+        <v>27</v>
       </c>
       <c r="H26">
-        <v>161936</v>
+        <v>230</v>
       </c>
       <c r="I26">
-        <v>12</v>
-      </c>
-      <c r="J26">
-        <v>1.2738130000000101</v>
+        <v>15</v>
+      </c>
+      <c r="J26" s="1">
+        <v>3.5544500000014502E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
       </c>
       <c r="E27">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F27">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G27">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H27">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="I27">
-        <v>15</v>
-      </c>
-      <c r="J27">
-        <v>3.5544500000014502E-2</v>
+        <v>18</v>
+      </c>
+      <c r="J27" s="1">
+        <v>4.2110000000320703E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1850,11 +4450,11 @@
       <c r="I28">
         <v>14</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="1">
         <v>1.5522167999999901</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1882,11 +4482,11 @@
       <c r="I29">
         <v>13</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="1">
         <v>0.94032929999980297</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1914,43 +4514,43 @@
       <c r="I30">
         <v>17</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="1">
         <v>7.4483477000001104</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
         <v>20</v>
       </c>
       <c r="E31">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="F31">
-        <v>7388</v>
+        <v>50</v>
       </c>
       <c r="G31">
-        <v>7390</v>
+        <v>52</v>
       </c>
       <c r="H31">
-        <v>65711</v>
+        <v>206</v>
       </c>
       <c r="I31">
-        <v>12</v>
-      </c>
-      <c r="J31">
-        <v>0.95949679999989701</v>
+        <v>6</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2.57154000000809E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1978,11 +4578,11 @@
       <c r="I32">
         <v>12</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="1">
         <v>17.2092408</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2010,11 +4610,11 @@
       <c r="I33">
         <v>12</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
         <v>153.93782929999901</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2042,11 +4642,11 @@
       <c r="I34">
         <v>12</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="1">
         <v>427.92823440000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2074,11 +4674,11 @@
       <c r="I35">
         <v>14</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="1">
         <v>4.94356599999991</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2106,75 +4706,75 @@
       <c r="I36">
         <v>24132</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
         <v>697.20993910000004</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E37">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="F37">
-        <v>113339</v>
+        <v>2467</v>
       </c>
       <c r="G37">
-        <v>113341</v>
+        <v>2469</v>
       </c>
       <c r="H37">
-        <v>1066413</v>
+        <v>22522</v>
       </c>
       <c r="I37">
-        <v>14</v>
-      </c>
-      <c r="J37">
-        <v>7.7705774000000902</v>
+        <v>9</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.612316599999985</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E38">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="F38">
-        <v>29</v>
+        <v>7388</v>
       </c>
       <c r="G38">
-        <v>31</v>
+        <v>7390</v>
       </c>
       <c r="H38">
-        <v>280</v>
+        <v>65711</v>
       </c>
       <c r="I38">
-        <v>18</v>
-      </c>
-      <c r="J38">
-        <v>4.2110000000320703E-2</v>
+        <v>12</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.95949679999989701</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2202,11 +4802,11 @@
       <c r="I39">
         <v>17</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="1">
         <v>2.2335081999999602</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2234,11 +4834,11 @@
       <c r="I40">
         <v>17</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="1">
         <v>1.8537143999997101</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2266,7 +4866,7 @@
       <c r="I41">
         <v>23</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="1">
         <v>28.852180499999999</v>
       </c>
     </row>
@@ -2298,11 +4898,11 @@
       <c r="I42">
         <v>14</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="1">
         <v>3.8185496999999402</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2330,11 +4930,11 @@
       <c r="I43">
         <v>15</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="1">
         <v>87.083080999999694</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2362,11 +4962,11 @@
       <c r="I44">
         <v>14</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="1">
         <v>1677.8132814999999</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2394,16 +4994,24 @@
       <c r="I45">
         <v>14</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="1">
         <v>4649.6154936999901</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J45" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J45">
-      <sortCondition ref="A1:A45"/>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="astar_search with h_unmet_goals"/>
+        <filter val="greedy_best_first_graph_search with h_unmet_goals"/>
+        <filter val="uniform_cost_search"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J42">
+      <sortCondition ref="B1:B45"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>